<commit_message>
Moved exelfile to planner-map
</commit_message>
<xml_diff>
--- a/planner/Överblick punkter.xlsx
+++ b/planner/Överblick punkter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffdb61f3ca5e596b/Gemensamma dokument/3.8. Skolan/WEBB-E-HANDEL/Courses/Systemutveckling 50 yhp och Databasteknik 20 yhp/Inlämningar/Webshop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffdb61f3ca5e596b/Gemensamma dokument/3.8. Skolan/WEBB-E-HANDEL/Repos/Webshop/diagrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="8_{A52E88B3-FB39-428B-99B6-AA879B0686C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D367F073-A625-4878-A728-E3982B4D6EBD}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{F6681498-EF8F-468A-B336-4973DBEDF5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34B63BED-4DB1-45D4-B889-6BF5847D09E5}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D4CAC9D2-5662-4D72-97CE-32DCF278DC94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <r>
       <t>1.</t>
@@ -154,12 +154,6 @@
       </rPr>
       <t>Det skall finnas en kortare text som beskriver erat projekt i er readme md (G)</t>
     </r>
-  </si>
-  <si>
-    <t>Kolla med Victor imorgon angående detta</t>
-  </si>
-  <si>
-    <t>Ingen ny produkt va? Som att skapa</t>
   </si>
   <si>
     <t>ALLMÄNT</t>
@@ -617,9 +611,6 @@
     </r>
   </si>
   <si>
-    <t>10.       En besökare ska kunna beställa produkter från sidan, detta ska uppdatera lagersaldot i databasen (G)</t>
-  </si>
-  <si>
     <r>
       <t>11.</t>
     </r>
@@ -762,23 +753,787 @@
     </r>
   </si>
   <si>
-    <t>Ex.</t>
-  </si>
-  <si>
-    <t>VerifyLogin(), loginAdmin();</t>
-  </si>
-  <si>
-    <t>SELECT email, password, FROM USER osv…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Behövs en loginsida. GET - skicka email och password </t>
+    <r>
+      <t xml:space="preserve">Hämta alla produkter </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT * FROM product</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Utifrån: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT INTO `subscriptionnews` (FirstName, LastName, Email) 
+VALUES ('Amina', 'Hallam', 'aminahallam@live.se')</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Med konto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> INSERT INTO subscriptionnews(UserID, FirstName, LastName, Email)
+SELECT UserID, FirstName, LastName, Email
+FROM user u
+where u.UserID = 1</t>
+    </r>
+  </si>
+  <si>
+    <t>Fixas med punkt 14?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skapa ett konto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> INSERT INTO user (Email, Password, FirstName, LastName, Street, CO, ZipCode, City, Country, CountryCode, StandardPhone,MobileNumber,Admin, TermsOfPurchase)
+VALUES ('grey@grey.se', 'ffefwfäfer', 'Per', 'Andersson', 'skitvägen', NULL, 12345, 'Malmö', 'Sweden', 46, NULL, 76123456, 0, 0)  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hämta lista med email + password:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SELECT Email, Password
+FROM `user`</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Uppdatera antal på produkt:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> UPDATE product p
+SET p.UnitsInStock = p.UnitsInStock +4
+WHERE p.productID = 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lista på alla subscribers:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SELECT * FROM `subscriptionnews`</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hämta efter kategori:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SELECT p.ProductID, c.CategoryID, c.CategoryName, p.Name, p.Description, p.UnitPrice, p.Image, p.UnitsInStock
+FROM productincategory pc
+JOIN product p
+	ON p.productid = pc.ProductID
+JOIN category c
+	ON c.CategoryID = pc.CategoryID
+WHERE c.CategoryID = 3</t>
+    </r>
+  </si>
+  <si>
+    <t>10.       En besökare ska kunna beställa produkter från sidan, detta ska uppdatera lagersaldot i databasen (G)   (Skapa order)</t>
+  </si>
+  <si>
+    <t>UPDATE productincategory pc
+SET pc.CategoryId =  1
+WHERE pc.CategoryId =  3 AND pc.productID = 5;</t>
+  </si>
+  <si>
+    <t>INSERT INTO newsletter VALUES(NULL, 'Min titel', 'brödtext', CURRENT_DATE)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skapa produkt:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> INSERT INTO `product` VALUES(NULL, 'Anka', '20 x 100', 3000, 10, 'anka.png')</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ge produkt en kategori:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> INSERT INTO productincategory VALUES(6, 3, CURRENT_DATE)  Kommentar: 6an skall vara variabeln på productID från skapandet av produkten. (productid, categoryid, lastupdated)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ta bort produkt:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DELETE
+FROM product
+WHERE productID = 22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Ge produkt en kategori: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> categoriID som value och namnet visualiserat.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ta bort produkt: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ID + Namn visualiserat (productID skickas som input till databasen)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skapa order:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> INSERT INTO `order` VALUES(NULL, 'REG', 1, 1, CURRENT_TIMESTAMP, NULL, NULL) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kommentar:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> variabel från userID, CourrierID)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lägg till produkt på order:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> INSERT INTO `orderdetails` VALUES(5, 7, 1); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kommentarer:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Alla values hämtas via variabler. Kan behöva loopas om det är fler produkter på en order. Skapa förutsättningar för det.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT CourrierID, CourrierName FROM `courrier` </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kommentar:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Spara ner CourrierID till en variabel. Skall användas på order.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Uppdatera UnitsInStock: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">UPDATE product p
+SET p.UnitsInStock = p.UnitsInStock -2
+WHERE p.productID = 5  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kommentar:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2an representerar variabeln för quantity.</t>
+    </r>
+  </si>
+  <si>
+    <t>När order skapas  och se punkt 20.</t>
+  </si>
+  <si>
+    <t>Punkt 22.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Överblick på gjroda ordrar för en kund</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: SELECT o.orderid, p.ProductID, p.Name, od.quantity, o.userid, o.registerDate, o.shippingDate, o.custrecdate, p.UnitPrice
+FROM `orderdetails` od
+JOIN `order` o 
+	ON o.orderid = od.orderid
+JOIN product p
+	ON p.ProductID = od.productid
+WHERE o.userid = 3    
+ORDER BY `orderid` ASC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hämta lista med email, password + admin:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SELECT Email, Password, admin
+FROM `user`</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lista på orders: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT o.orderid, o.statusid, u.FirstName, u.LastName, c.CourrierName, o.registerdate, o.shippingdate, o.custrecdate
+FROM `order` o
+	JOIN user u
+    ON u.UserID = o.userid
+    JOIN courrier c
+    ON c.CourrierID = o.courrierID</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Totalsumma på orderrader:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SELECT od.orderid, od.productid, p.Name, od.quantity, od.quantity * p.UnitPrice AS 'Totalsumma' FROM `orderdetails` od JOIN product p ON p.ProductID = od.productid ORDER BY `orderid` ASC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Totalsumma på ordrar: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT od.orderid, SUM(od.quantity * p.UnitPrice) AS 'Totalsum' FROM `orderdetails` od JOIN product p ON p.ProductID = od.productid GROUP BY od.orderid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Överblick på mottagna ordrar:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SELECT o.orderid, o.statusid, u.FirstName, u.LastName, c.CourrierName, o.registerdate, o.shippingdate, o.custrecdate
+FROM `order` o
+	JOIN user u
+    ON u.UserID = o.userid
+    JOIN courrier c
+    ON c.CourrierID = o.courrierID
+    WHERE o.statusid = 'crec'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Markera beställning som skickad: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UPDATE `order`
+SET statusid = 'SHIP', ShippingDate = CURRENT_TIMESTAMP , CustRecDate = NULL
+WHERE orderid = 6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Överblick på registrerade ordrar:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SELECT o.orderid, o.statusid, u.FirstName, u.LastName, c.CourrierName, o.registerdate, o.shippingdate, o.custrecdate
+FROM `order` o
+	JOIN user u
+    ON u.UserID = o.userid
+    JOIN courrier c
+    ON c.CourrierID = o.courrierID
+    WHERE o.statusid = 'reg'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Överblick på registrerade ordrar med filtrering på user eller order:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SELECT o.orderid, o.statusid, u.FirstName, u.LastName, c.CourrierName, o.registerdate, o.shippingdate, o.custrecdate
+FROM `order` o
+	JOIN user u
+    ON u.UserID = o.userid
+    JOIN courrier c
+    ON c.CourrierID = o.courrierID
+    WHERE o.orderid = NULL OR u.UserID = 2 AND StatusID = 'reg'</t>
+    </r>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Victor går igenom detta</t>
+  </si>
+  <si>
+    <t>Uppdatera orderstatus: UPDATE `order`
+SET StatusID = 'CREC', CustRecDate = CURRENT_TIMESTAMP
+WHERE OrderID = 5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nytt alternativ på överblick:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SELECT o.orderid, o.statusid, c.CourrierName, o.registerdate, o.shippingdate, o.custrecdate, os.Description
+FROM `order` o
+	JOIN user u
+    ON u.UserID = o.userid
+    JOIN courrier c
+    ON c.CourrierID = o.courrierID
+    JOIN orderstatus os
+    ON os.StatusID = o.statusID
+    WHERE u.UserID = 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Skapa produkt: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Name, Description, UnitPrice, UnitsInStock, Image  </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,8 +1573,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -834,12 +1603,28 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -982,11 +1767,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1006,24 +1952,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1063,11 +1991,172 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bra" xfId="1" builtinId="26"/>
+    <cellStyle name="Dålig" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1380,384 +2469,585 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0A3FD6-5A19-4844-88AD-0B477651B241}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="167.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="21" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="149.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" style="62" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="62" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" style="62" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="F1" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="63"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="65"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="65"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="61"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="61"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="68"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="68"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="59"/>
+    </row>
+    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="70" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="65"/>
+    </row>
+    <row r="19" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="65"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
+    </row>
+    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="65"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="64"/>
+      <c r="G22" s="65"/>
+    </row>
+    <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="64"/>
+      <c r="G23" s="65"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="60"/>
+      <c r="G24" s="61"/>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="68"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="64"/>
+      <c r="H28" s="18"/>
+    </row>
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="1:8" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="63"/>
+    </row>
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="B33" s="11"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="18"/>
+    </row>
+    <row r="35" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="41"/>
+      <c r="C37" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="48"/>
+      <c r="E37" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="55"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="48"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="56"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="48"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="18"/>
+    </row>
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="40"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="F40" s="64"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41" s="64"/>
+      <c r="G41" s="64"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A42" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="24"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="18"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="24"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" s="26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="24"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="24"/>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="24"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="24"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="B44" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="24"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="24"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="20"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="14"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E45" s="63"/>
+      <c r="F45" s="63"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>